<commit_message>
Updates for new data
</commit_message>
<xml_diff>
--- a/public_data/Translations.xlsx
+++ b/public_data/Translations.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
   <si>
     <t>Sheet</t>
   </si>
@@ -276,6 +276,15 @@
   </si>
   <si>
     <t>Léky</t>
+  </si>
+  <si>
+    <t>Jiný lék na Covid/plaquenil</t>
+  </si>
+  <si>
+    <t>Hydroxychloroquine</t>
+  </si>
+  <si>
+    <t>Jiný lék na Covid-plaquenil</t>
   </si>
 </sst>
 </file>
@@ -350,57 +359,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color auto="1"/>
@@ -831,7 +790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>34</v>
       </c>
@@ -839,7 +798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -855,7 +814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
@@ -863,7 +822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
@@ -871,7 +830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -911,7 +870,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
@@ -927,7 +886,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>44</v>
       </c>
@@ -935,7 +894,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>45</v>
       </c>
@@ -975,7 +934,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -983,7 +942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -991,7 +950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -999,7 +958,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
@@ -1007,7 +966,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
@@ -1015,7 +974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>51</v>
       </c>
@@ -1174,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,6 +1200,22 @@
         <v>85</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>